<commit_message>
added excel function supporting dfs, rows, cols
</commit_message>
<xml_diff>
--- a/results/ML/SLR_MotherEd_vs_S2_GRD_2TO29/evaluateRegModel.xlsx
+++ b/results/ML/SLR_MotherEd_vs_S2_GRD_2TO29/evaluateRegModel.xlsx
@@ -375,65 +375,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
+      <c r="D2">
         <v>0.2926829268292683</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
+      <c r="E2">
         <v>0.03448275862068965</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
+      <c r="F2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
+      <c r="G2">
         <v>0.06451612903225806</v>
       </c>
     </row>

</xml_diff>